<commit_message>
initial functionality and testing of cleanImport completed
</commit_message>
<xml_diff>
--- a/tests/testthat/ages.xlsx
+++ b/tests/testthat/ages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/erobin17_calpoly_edu/Documents/stat-331-calpoly/check-ins/2.1-loading-data/Ages_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/stodd03_calpoly_edu/Documents/Year3-2022-2023/3-Spring/STAT-431/DataAnalyzeR/tests/testthat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_442612902C2A016AF31AA89CB822D77F19303EF5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48505D8A-7D79-4098-AA31-4B8E66DDB53B}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_442612902C2A016AF31AA89CB822D77F19303EF5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67771DEE-858E-4698-A0FF-415CB3BCE0D3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="528" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Timo</t>
+  </si>
+  <si>
+    <t>Bob</t>
   </si>
 </sst>
 </file>
@@ -853,11 +856,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B636B24-8AAE-4603-A05C-9759E08D0BFD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -865,13 +868,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -879,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -887,7 +892,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -895,7 +900,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -903,7 +908,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -911,20 +916,25 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>25</v>
-      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>